<commit_message>
show speciel colums and hide
</commit_message>
<xml_diff>
--- a/php/products.xlsx
+++ b/php/products.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -41,10 +41,13 @@
     <t>Katzenkiste</t>
   </si>
   <si>
+    <t>Fahrrad</t>
+  </si>
+  <si>
     <t>Fressen</t>
   </si>
   <si>
-    <t>Ball</t>
+    <t>Katzentoilette</t>
   </si>
   <si>
     <t>Halsband</t>
@@ -62,7 +65,7 @@
     <t>zum kacken</t>
   </si>
   <si>
-    <t>Katzentoilette</t>
+    <t>sfasdfsdfadsafd</t>
   </si>
   <si>
     <t>Anzahl der Produkte:</t>
@@ -581,7 +584,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,44 +641,44 @@
         <v>8</v>
       </c>
       <c r="B3" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C3" s="6">
-        <v>2.5</v>
+        <v>0.0</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>9</v>
-      </c>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" customHeight="1" ht="20">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
-        <v>9.99</v>
+        <v>2.5</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6" customHeight="1" ht="20">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C5" s="6">
-        <v>10.5</v>
+        <v>9.99</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
@@ -688,10 +691,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3">
-        <v>0.0</v>
+        <v>10.5</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -707,46 +710,62 @@
         <v>0</v>
       </c>
       <c r="C7" s="6">
-        <v>29.99</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" customHeight="1" ht="20">
+      <c r="A8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>29.99</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" customHeight="1" ht="25">
-      <c r="A8" s="10" t="s">
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" s="18">
+    </row>
+    <row r="9" spans="1:6" customHeight="1" ht="25">
+      <c r="A9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9" s="18">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" customHeight="1" ht="25">
-      <c r="A9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="19">
+    <row r="10" spans="1:6" customHeight="1" ht="25">
+      <c r="A10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="19">
         <v>339</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A8:E8"/>
     <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
show update table by switch column
</commit_message>
<xml_diff>
--- a/php/products.xlsx
+++ b/php/products.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Fahrrad</t>
+  </si>
+  <si>
+    <t>Keller</t>
   </si>
   <si>
     <t>Fressen</t>
@@ -584,7 +587,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -654,47 +657,47 @@
     </row>
     <row r="4" spans="1:6" customHeight="1" ht="20">
       <c r="A4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>2.5</v>
+        <v>20.0</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" customHeight="1" ht="20">
       <c r="A5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6">
-        <v>9.99</v>
+        <v>2.5</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="17" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:6" customHeight="1" ht="20">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3">
-        <v>10.5</v>
+        <v>9.99</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -707,10 +710,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="5">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6">
-        <v>0.0</v>
+        <v>10.5</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
@@ -726,46 +729,62 @@
         <v>0</v>
       </c>
       <c r="C8" s="3">
-        <v>29.99</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" customHeight="1" ht="20">
+      <c r="A9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>29.99</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" customHeight="1" ht="25">
-      <c r="A9" s="10" t="s">
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9" s="18">
-        <v>41</v>
-      </c>
     </row>
     <row r="10" spans="1:6" customHeight="1" ht="25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="19">
-        <v>339</v>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10" s="18">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" customHeight="1" ht="25">
+      <c r="A11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="19">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A9:E9"/>
     <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>